<commit_message>
Merge with Jobstreet Process, Bug Fixing and some Improvements
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57da4d74ddf3ad5c/Documents/UiPath/ReFrameWork/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{4C6F0680-7CBF-4976-9863-5109C4AA17F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F64F0C5B-ADC4-49A8-8581-06C3528FCF94}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{4C6F0680-7CBF-4976-9863-5109C4AA17F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89B00F07-6FD6-44ED-9032-0FB3F70C8ADA}"/>
   <bookViews>
-    <workbookView xWindow="3336" yWindow="3396" windowWidth="19704" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3336" yWindow="3396" windowWidth="19704" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -119,10 +119,13 @@
     <t>resultPath</t>
   </si>
   <si>
-    <t>Kalibrr Talent Requirement</t>
+    <t>applicationsToClose</t>
   </si>
   <si>
-    <t>applicationsToClose</t>
+    <t>kalibrrUrl</t>
+  </si>
+  <si>
+    <t>Talent Requirement</t>
   </si>
 </sst>
 </file>
@@ -494,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -545,7 +548,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>28</v>
@@ -2678,8 +2681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2734,13 +2737,20 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>